<commit_message>
wylaczenie automatyczngo wypelniania w rejestracji konta
</commit_message>
<xml_diff>
--- a/wwwroot/Oferta.xlsx
+++ b/wwwroot/Oferta.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>Oferta z dnia: 28.02.2023</x:t>
+    <x:t>Oferta z dnia: 15.10.2023</x:t>
   </x:si>
   <x:si>
     <x:t>Tel. kom.: (+48 61) 694 160 741 
@@ -48,20 +48,65 @@
     <x:t>WARTOŚĆ POZYCJI BRUTTO</x:t>
   </x:si>
   <x:si>
-    <x:t>A01502</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Lampion ABBASI exclusive design XXL_Aluro 
-Szerokość: 38,00 cm 
-Głębokość: 38,00 cm 
-Wysokość: 115,00 cm 
+    <x:t>A01655</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Gwiazdka wisząca NATURE_Aluro L 
+Szerokość: 23,00 cm 
+Głębokość: 4,00 cm 
+Wysokość: 23,00 cm 
 </x:t>
   </x:si>
   <x:si>
-    <x:t>850,00 zł</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1/1 szt.</x:t>
+    <x:t>11,80 zł</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/6 szt.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A01656</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Gwiazdka wisząca NATURE_Aluro XL 
+Szerokość: 32,00 cm 
+Głębokość: 5,00 cm 
+Wysokość: 32,00 cm 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17,90 zł</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/4 szt.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A01670</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Renifer stojący_Aluro XL 
+Szerokość: 32,00 cm 
+Głębokość: 5,00 cm 
+Wysokość: 29,00 cm 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76,00 zł</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/8 szt.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A01667</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Renifer świecznik_Aluro 
+Szerokość: 22,00 cm 
+Głębokość: 10,00 cm 
+Wysokość: 23,00 cm 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32,90 zł</x:t>
   </x:si>
   <x:si>
     <x:t>WARTOŚĆ ZAMÓWIENIA</x:t>
@@ -129,7 +174,7 @@
       </x:patternFill>
     </x:fill>
   </x:fills>
-  <x:borders count="4">
+  <x:borders count="5">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -174,7 +219,7 @@
       <x:top style="thin">
         <x:color rgb="FF000000"/>
       </x:top>
-      <x:bottom style="thick">
+      <x:bottom style="thin">
         <x:color rgb="FF000000"/>
       </x:bottom>
       <x:diagonal style="none">
@@ -198,8 +243,25 @@
         <x:color rgb="FF000000"/>
       </x:diagonal>
     </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="thin">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="thick">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="11">
+  <x:cellStyleXfs count="13">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -227,6 +289,12 @@
     <x:xf numFmtId="164" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -234,7 +302,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="14">
+  <x:cellXfs count="17">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -280,6 +348,18 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -325,37 +405,6 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="2381250" cy="1162050"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect"/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1619250" cy="1619250"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId7" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1619250" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>
@@ -653,7 +702,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:O5"/>
+  <x:dimension ref="A1:O8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
       <x:pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
@@ -770,17 +819,23 @@
       <x:c r="N4" s="2"/>
       <x:c r="O4" s="2"/>
     </x:row>
-    <x:row r="5" spans="1:15" ht="30" customHeight="1">
-      <x:c r="A5" s="1"/>
-      <x:c r="B5" s="2"/>
-      <x:c r="C5" s="2"/>
-      <x:c r="D5" s="2"/>
-      <x:c r="E5" s="2"/>
-      <x:c r="F5" s="12" t="s">
+    <x:row r="5" spans="1:15" ht="130" customHeight="1">
+      <x:c r="A5" s="8"/>
+      <x:c r="B5" s="9" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="G5" s="13">
-        <x:f>SUM(G4:G4)</x:f>
+      <x:c r="C5" s="9" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D5" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E5" s="9" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F5" s="9" t="s"/>
+      <x:c r="G5" s="11">
+        <x:f>D5*F5</x:f>
       </x:c>
       <x:c r="H5" s="2"/>
       <x:c r="I5" s="2"/>
@@ -790,6 +845,81 @@
       <x:c r="M5" s="2"/>
       <x:c r="N5" s="2"/>
       <x:c r="O5" s="2"/>
+    </x:row>
+    <x:row r="6" spans="1:15" ht="130" customHeight="1">
+      <x:c r="A6" s="8"/>
+      <x:c r="B6" s="9" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C6" s="9" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D6" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E6" s="9" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F6" s="9" t="s"/>
+      <x:c r="G6" s="11">
+        <x:f>D6*F6</x:f>
+      </x:c>
+      <x:c r="H6" s="2"/>
+      <x:c r="I6" s="2"/>
+      <x:c r="J6" s="2"/>
+      <x:c r="K6" s="2"/>
+      <x:c r="L6" s="2"/>
+      <x:c r="M6" s="2"/>
+      <x:c r="N6" s="2"/>
+      <x:c r="O6" s="2"/>
+    </x:row>
+    <x:row r="7" spans="1:15" ht="130" customHeight="1">
+      <x:c r="A7" s="12"/>
+      <x:c r="B7" s="13" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C7" s="13" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D7" s="14" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E7" s="13" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F7" s="13" t="s"/>
+      <x:c r="G7" s="11">
+        <x:f>D7*F7</x:f>
+      </x:c>
+      <x:c r="H7" s="2"/>
+      <x:c r="I7" s="2"/>
+      <x:c r="J7" s="2"/>
+      <x:c r="K7" s="2"/>
+      <x:c r="L7" s="2"/>
+      <x:c r="M7" s="2"/>
+      <x:c r="N7" s="2"/>
+      <x:c r="O7" s="2"/>
+    </x:row>
+    <x:row r="8" spans="1:15" ht="30" customHeight="1">
+      <x:c r="A8" s="1"/>
+      <x:c r="B8" s="2"/>
+      <x:c r="C8" s="2"/>
+      <x:c r="D8" s="2"/>
+      <x:c r="E8" s="2"/>
+      <x:c r="F8" s="15" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G8" s="16">
+        <x:f>SUM(G4:G7)</x:f>
+      </x:c>
+      <x:c r="H8" s="2"/>
+      <x:c r="I8" s="2"/>
+      <x:c r="J8" s="2"/>
+      <x:c r="K8" s="2"/>
+      <x:c r="L8" s="2"/>
+      <x:c r="M8" s="2"/>
+      <x:c r="N8" s="2"/>
+      <x:c r="O8" s="2"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="2">

</xml_diff>